<commit_message>
multiples UFRC code drafted
</commit_message>
<xml_diff>
--- a/documents/datadictionary/perinatal_ICD_codes_rawdata_01_2022.xlsx
+++ b/documents/datadictionary/perinatal_ICD_codes_rawdata_01_2022.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a87caf6b30614cd/Documents/ehr-preeclampsia-model/documents/datadictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A4005AD1-E51A-4BCE-8F8B-DFD95862EFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:40009_{A4005AD1-E51A-4BCE-8F8B-DFD95862EFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A75E3964-665D-43A8-8636-05FBD4F42700}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
+    <workbookView xWindow="31860" yWindow="405" windowWidth="15375" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="perinatal_ICD_codes_rawdata_01_" sheetId="1" r:id="rId1"/>
-    <sheet name="multiples" sheetId="2" r:id="rId2"/>
+    <sheet name="multiples" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6549" uniqueCount="3737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6560" uniqueCount="3748">
   <si>
     <t>perinatal_dx_code</t>
   </si>
@@ -11232,12 +11232,45 @@
   </si>
   <si>
     <t>antepartum</t>
+  </si>
+  <si>
+    <t>651.93</t>
+  </si>
+  <si>
+    <t>651.33</t>
+  </si>
+  <si>
+    <t>651.31</t>
+  </si>
+  <si>
+    <t>651.63</t>
+  </si>
+  <si>
+    <t>651.83</t>
+  </si>
+  <si>
+    <t>651.8</t>
+  </si>
+  <si>
+    <t>651.81</t>
+  </si>
+  <si>
+    <t>651.2</t>
+  </si>
+  <si>
+    <t>651.7</t>
+  </si>
+  <si>
+    <t>651.43</t>
+  </si>
+  <si>
+    <t>651.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -11715,11 +11748,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -12074,10 +12108,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2290"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D79"/>
     </sheetView>
   </sheetViews>
@@ -37526,16 +37560,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25322A42-3D14-40A9-B143-7C3722FBA2B5}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
@@ -37544,1586 +37578,1587 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>3723</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>3724</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3730</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1536</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>3722</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>3725</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>3731</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>1537</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>1751</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>3722</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>3725</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>3732</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>1752</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>1755</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>3722</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>3725</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>3733</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>1756</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>1757</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>3722</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>3725</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>3732</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>1758</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>1763</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>3722</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>3725</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>3735</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>1764</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>1771</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>3722</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>3725</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>3734</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>1772</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>2019</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>3722</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>3725</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>3733</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>2020</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>2079</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>3722</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>3725</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>3734</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>2080</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>2087</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>3722</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>3725</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>3735</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>2088</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>2089</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>3722</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>3725</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>3734</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>2090</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>2091</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>3722</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>3725</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>3733</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>2092</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>2093</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>3722</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>3725</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>3735</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>2094</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>2097</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>3722</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>3725</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>3732</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>2098</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>2140</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>3722</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>3725</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>3735</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>2141</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>2142</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>3722</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>3725</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>3732</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>2143</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>2158</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>3722</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>3725</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>3732</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>2159</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>2239</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>3722</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>3725</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>3735</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>2240</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>2241</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>3722</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>3726</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>3735</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>2242</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>2287</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>3722</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>3727</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>3734</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>2288</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>2289</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>3722</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>3727</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>3734</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>2290</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>2293</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>3722</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>3727</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>3733</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>2294</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>2295</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>3722</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>3725</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>3733</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>2296</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>2346</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>3722</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>3726</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>3734</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>2347</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>2555</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>3722</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>3726</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>3733</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>2556</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>2656</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>3722</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>3725</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>3734</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>2657</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>2766</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>3722</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>3727</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>3735</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>2767</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>2768</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>3722</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>3727</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>3732</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>2769</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>2770</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>3722</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>3727</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>3732</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>2771</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>2772</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>3722</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>3727</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" t="s">
         <v>3733</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>2773</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>2806</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>3722</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>3727</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>3732</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>2807</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F31" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>2914</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>3722</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>3726</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>3732</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>2915</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="F32" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>3135</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>3722</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>3728</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>3732</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>3136</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F33" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>3248</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>3722</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>3727</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>3735</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>3249</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
         <v>3250</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>3722</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>3727</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" t="s">
         <v>3735</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>3251</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>3252</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>3722</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>3727</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" t="s">
         <v>3734</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>3253</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="F36" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="2" t="s">
         <v>3254</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>3722</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>3727</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" t="s">
         <v>3735</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>3255</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="F37" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>3412</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>3722</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>3728</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" t="s">
         <v>3735</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>3413</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="F38" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="2" t="s">
         <v>3414</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>3722</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>3728</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" t="s">
         <v>3735</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>3415</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F39" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>3416</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>3722</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>3728</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>3733</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>3417</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="F40" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>3418</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>3722</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>3728</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" t="s">
         <v>3735</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>3419</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="F41" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>3422</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>3722</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>3728</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" t="s">
         <v>3733</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>3423</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="F42" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="2" t="s">
         <v>3424</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>3722</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>3728</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" t="s">
         <v>3732</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>3425</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F43" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
         <v>3428</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>3722</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>3727</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" t="s">
         <v>3732</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>3429</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="2" t="s">
         <v>3430</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>3722</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" t="s">
         <v>3727</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" t="s">
         <v>3733</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>3431</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>3472</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>3722</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>3725</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" t="s">
         <v>3732</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>3473</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="F46" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="2" t="s">
         <v>3504</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>3722</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>3727</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" t="s">
         <v>3734</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>3505</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>3550</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>3722</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" t="s">
         <v>3725</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" t="s">
         <v>3735</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>3551</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="2" t="s">
         <v>3552</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>3722</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>3725</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="D49" t="s">
         <v>3734</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>3553</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F49" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>3602</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>3722</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>3728</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" t="s">
         <v>3734</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" t="s">
         <v>3603</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="F50" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="2" t="s">
         <v>3626</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>3722</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" t="s">
         <v>3729</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" t="s">
         <v>3734</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" t="s">
         <v>3627</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>3636</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>3722</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>3725</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" t="s">
         <v>3733</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E52" t="s">
         <v>3637</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="F52" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="2" t="s">
         <v>3680</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>3722</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" t="s">
         <v>3727</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" t="s">
         <v>3735</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" t="s">
         <v>3681</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="F53" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="2" t="s">
         <v>3708</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>3722</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" t="s">
         <v>3727</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" t="s">
         <v>3733</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E54" t="s">
         <v>3709</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="F54" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="2" t="s">
         <v>3710</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>3722</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" t="s">
         <v>3727</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" t="s">
         <v>3734</v>
       </c>
-      <c r="E55" s="1" t="s">
+      <c r="E55" t="s">
         <v>3711</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="F55" t="s">
         <v>856</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="A56" s="2">
         <v>651.03</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>3722</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" t="s">
         <v>3725</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" t="s">
         <v>3736</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E56" t="s">
         <v>40</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="F56" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+      <c r="A57" s="2">
         <v>651.01</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>3722</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" t="s">
         <v>3725</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" t="s">
         <v>3736</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" t="s">
         <v>112</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="F57" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="A58" s="2">
         <v>651</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>3722</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" t="s">
         <v>3725</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" t="s">
         <v>3733</v>
       </c>
-      <c r="E58" s="1" t="s">
+      <c r="E58" t="s">
         <v>113</v>
       </c>
-      <c r="F58" s="1" t="s">
+      <c r="F58" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
-        <v>651.92999999999995</v>
-      </c>
-      <c r="B59" s="1" t="s">
+      <c r="A59" s="2" t="s">
+        <v>3737</v>
+      </c>
+      <c r="B59" t="s">
         <v>3722</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" t="s">
         <v>3726</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" t="s">
         <v>3733</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E59" t="s">
         <v>156</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F59" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+      <c r="A60" s="2">
         <v>651.9</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>3722</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" t="s">
         <v>3726</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" t="s">
         <v>3733</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" t="s">
         <v>290</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F60" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
-        <v>651.33000000000004</v>
-      </c>
-      <c r="B61" s="1" t="s">
+      <c r="A61" s="2" t="s">
+        <v>3738</v>
+      </c>
+      <c r="B61" t="s">
         <v>3722</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" t="s">
         <v>3725</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" t="s">
         <v>3733</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E61" t="s">
         <v>432</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="F61" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
-        <v>651.30999999999995</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="A62" s="2" t="s">
+        <v>3739</v>
+      </c>
+      <c r="B62" t="s">
         <v>3722</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" t="s">
         <v>3725</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" t="s">
         <v>3733</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E62" t="s">
         <v>433</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="F62" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>651.63</v>
-      </c>
-      <c r="B63" s="1" t="s">
+      <c r="A63" s="2" t="s">
+        <v>3740</v>
+      </c>
+      <c r="B63" t="s">
         <v>3722</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" t="s">
         <v>3726</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" t="s">
         <v>3733</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="E63" t="s">
         <v>434</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
-        <v>651.83000000000004</v>
-      </c>
-      <c r="B64" s="1" t="s">
+      <c r="A64" s="2" t="s">
+        <v>3741</v>
+      </c>
+      <c r="B64" t="s">
         <v>3722</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" t="s">
         <v>3726</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" t="s">
         <v>3733</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E64" t="s">
         <v>459</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+      <c r="A65" s="2">
         <v>651.61</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
         <v>3722</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" t="s">
         <v>3726</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" t="s">
         <v>3733</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" t="s">
         <v>474</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="F65" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+      <c r="A66" s="2">
         <v>651.1</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" t="s">
         <v>3722</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" t="s">
         <v>3727</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" t="s">
         <v>3733</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E66" t="s">
         <v>550</v>
       </c>
-      <c r="F66" s="1" t="s">
+      <c r="F66" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+      <c r="A67" s="2">
         <v>651.11</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
         <v>3722</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" t="s">
         <v>3727</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" t="s">
         <v>3733</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" t="s">
         <v>551</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="F67" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+      <c r="A68" s="2">
         <v>651.23</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>3722</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" t="s">
         <v>3728</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" t="s">
         <v>3733</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E68" t="s">
         <v>583</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="F68" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+      <c r="A69" s="2">
         <v>651.13</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" t="s">
         <v>3722</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" t="s">
         <v>3727</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" t="s">
         <v>3733</v>
       </c>
-      <c r="E69" s="1" t="s">
+      <c r="E69" t="s">
         <v>614</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="F69" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+      <c r="A70" s="2">
         <v>651.21</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" t="s">
         <v>3722</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" t="s">
         <v>3728</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" t="s">
         <v>3733</v>
       </c>
-      <c r="E70" s="1" t="s">
+      <c r="E70" t="s">
         <v>711</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="F70" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
-        <v>651.79999999999995</v>
-      </c>
-      <c r="B71" s="1" t="s">
+      <c r="A71" s="2" t="s">
+        <v>3742</v>
+      </c>
+      <c r="B71" t="s">
         <v>3722</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" t="s">
         <v>3726</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" t="s">
         <v>3733</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" t="s">
         <v>735</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="F71" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>651.80999999999995</v>
-      </c>
-      <c r="B72" s="1" t="s">
+      <c r="A72" s="2" t="s">
+        <v>3743</v>
+      </c>
+      <c r="B72" t="s">
         <v>3722</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" t="s">
         <v>3726</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" t="s">
         <v>3733</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" t="s">
         <v>742</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="F72" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+      <c r="A73" s="2">
         <v>651.91</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" t="s">
         <v>3722</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" t="s">
         <v>3726</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" t="s">
         <v>3733</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E73" t="s">
         <v>759</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F73" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
-        <v>651.20000000000005</v>
-      </c>
-      <c r="B74" s="1" t="s">
+      <c r="A74" s="2" t="s">
+        <v>3744</v>
+      </c>
+      <c r="B74" t="s">
         <v>3722</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" t="s">
         <v>3728</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" t="s">
         <v>3733</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" t="s">
         <v>799</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F74" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+      <c r="A75" s="2">
         <v>651.41</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>3722</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" t="s">
         <v>3727</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" t="s">
         <v>3733</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" t="s">
         <v>802</v>
       </c>
-      <c r="F75" s="1" t="s">
+      <c r="F75" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>651.70000000000005</v>
-      </c>
-      <c r="B76" s="1" t="s">
+      <c r="A76" s="2" t="s">
+        <v>3745</v>
+      </c>
+      <c r="B76" t="s">
         <v>3722</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" t="s">
         <v>3726</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D76" t="s">
         <v>3733</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E76" t="s">
         <v>818</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="F76" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+      <c r="A77" s="2">
         <v>651.71</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" t="s">
         <v>3722</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" t="s">
         <v>3726</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D77" t="s">
         <v>3733</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" t="s">
         <v>819</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F77" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>651.42999999999995</v>
-      </c>
-      <c r="B78" s="1" t="s">
+      <c r="A78" s="2" t="s">
+        <v>3746</v>
+      </c>
+      <c r="B78" t="s">
         <v>3722</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" t="s">
         <v>3727</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D78" t="s">
         <v>3733</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E78" t="s">
         <v>820</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="F78" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>651.29999999999995</v>
-      </c>
-      <c r="B79" s="1" t="s">
+      <c r="A79" s="2" t="s">
+        <v>3747</v>
+      </c>
+      <c r="B79" t="s">
         <v>3722</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" t="s">
         <v>3725</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D79" t="s">
         <v>3733</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E79" t="s">
         <v>848</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F79" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to hypertension and diabetes codes
</commit_message>
<xml_diff>
--- a/documents/datadictionary/perinatal_ICD_codes_rawdata_01_2022.xlsx
+++ b/documents/datadictionary/perinatal_ICD_codes_rawdata_01_2022.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a87caf6b30614cd/Documents/ehr-preeclampsia-model/documents/datadictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="306" documentId="13_ncr:40009_{A4005AD1-E51A-4BCE-8F8B-DFD95862EFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{272C8207-8010-4B08-B8AF-57A50A1D0151}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9024541E-BFC9-4B55-8A8E-040948A85B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="900" windowWidth="21360" windowHeight="14220" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="perinatal_ICD_codes_rawdata_01" sheetId="1" r:id="rId1"/>
-    <sheet name="hypertension" sheetId="6" r:id="rId2"/>
-    <sheet name="diabetes" sheetId="7" r:id="rId3"/>
+    <sheet name="diabetes" sheetId="7" r:id="rId2"/>
+    <sheet name="hypertension" sheetId="6" r:id="rId3"/>
     <sheet name="multiples" sheetId="3" r:id="rId4"/>
     <sheet name="pe" sheetId="5" r:id="rId5"/>
     <sheet name="pulmonary" sheetId="9" r:id="rId6"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7518" uniqueCount="3767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7517" uniqueCount="3766">
   <si>
     <t>perinatal_dx_code</t>
   </si>
@@ -11323,9 +11323,6 @@
   </si>
   <si>
     <t>pulmonary</t>
-  </si>
-  <si>
-    <t>642.2</t>
   </si>
 </sst>
 </file>
@@ -11468,7 +11465,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11648,6 +11645,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -11809,13 +11812,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -12176,7 +12182,7 @@
   <dimension ref="A1:D2290"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A169" sqref="A1:XFD1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38098,1081 +38104,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E6D65C-6D8A-4E42-AF7B-9ACBFC461D1A}">
-  <dimension ref="A1:F58"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="146" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3723</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3724</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3730</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>642</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>642.01</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>642.02</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>642.03</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>642.04</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>642.11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>642.13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>642.14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>849</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>3766</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>642.21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>642.23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>642.24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>642.29999999999995</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>642.30999999999995</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>642.32000000000005</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>642.33000000000004</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>642.34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>642.9</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>642.91</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>642.91999999999996</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>642.92999999999995</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>642.94000000000005</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>1236</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1" t="s">
-        <v>1237</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>993</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1" t="s">
-        <v>994</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>933</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1" t="s">
-        <v>934</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>957</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1" t="s">
-        <v>958</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>1120</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1" t="s">
-        <v>1121</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>1297</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1" t="s">
-        <v>1298</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>2678</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1" t="s">
-        <v>2679</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>1341</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1" t="s">
-        <v>1342</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>2798</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1" t="s">
-        <v>2799</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>2299</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1" t="s">
-        <v>2300</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>2752</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1" t="s">
-        <v>2753</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>3290</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1" t="s">
-        <v>3291</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1" t="s">
-        <v>1235</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>1345</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1" t="s">
-        <v>1346</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>1003</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1" t="s">
-        <v>1004</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>919</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1" t="s">
-        <v>920</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>1023</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1" t="s">
-        <v>1024</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>925</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>2336</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1" t="s">
-        <v>2337</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>1439</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1" t="s">
-        <v>1440</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>921</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1" t="s">
-        <v>922</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>1150</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1" t="s">
-        <v>1151</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>1401</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1" t="s">
-        <v>1402</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>947</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1" t="s">
-        <v>948</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>1240</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1" t="s">
-        <v>1241</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>1682</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1" t="s">
-        <v>1683</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>883</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1" t="s">
-        <v>884</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>854</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1" t="s">
-        <v>855</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>1353</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1" t="s">
-        <v>1354</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1" t="s">
-        <v>1714</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1" t="s">
-        <v>1231</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>1009</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1" t="s">
-        <v>1010</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>1162</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1" t="s">
-        <v>1163</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>1248</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1" t="s">
-        <v>1249</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>929</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1" t="s">
-        <v>930</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3321D195-85F5-451B-BB8A-48DC8CAF4B8E}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39212,8 +38148,8 @@
       <c r="B2" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>3763</v>
+      <c r="C2" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
@@ -39230,8 +38166,8 @@
       <c r="B3" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>3763</v>
+      <c r="C3" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
@@ -39626,8 +38562,8 @@
       <c r="B25" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>3763</v>
+      <c r="C25" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
@@ -39644,8 +38580,8 @@
       <c r="B26" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>3763</v>
+      <c r="C26" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
@@ -39662,8 +38598,8 @@
       <c r="B27" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>3763</v>
+      <c r="C27" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
@@ -39680,8 +38616,8 @@
       <c r="B28" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>3763</v>
+      <c r="C28" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
@@ -39698,8 +38634,8 @@
       <c r="B29" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>3763</v>
+      <c r="C29" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
@@ -39716,8 +38652,8 @@
       <c r="B30" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>3763</v>
+      <c r="C30" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
@@ -39734,8 +38670,8 @@
       <c r="B31" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>3763</v>
+      <c r="C31" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
@@ -39752,8 +38688,8 @@
       <c r="B32" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>3763</v>
+      <c r="C32" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
@@ -39770,8 +38706,8 @@
       <c r="B33" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>3763</v>
+      <c r="C33" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
@@ -39788,8 +38724,8 @@
       <c r="B34" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>3763</v>
+      <c r="C34" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
@@ -39806,8 +38742,8 @@
       <c r="B35" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>3763</v>
+      <c r="C35" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
@@ -39824,8 +38760,8 @@
       <c r="B36" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>3763</v>
+      <c r="C36" s="4" t="s">
+        <v>3762</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
@@ -40048,6 +38984,1075 @@
         <v>1308</v>
       </c>
       <c r="F48" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E6D65C-6D8A-4E42-AF7B-9ACBFC461D1A}">
+  <dimension ref="A1:F58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="146" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3723</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3724</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3730</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>642</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>642.01</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>642.02</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>642.03</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>642.04</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>642.11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>642.13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>642.14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>642.20000000000005</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>642.21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>642.23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>642.24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>642.29999999999995</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>642.30999999999995</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>642.32000000000005</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>642.33000000000004</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>642.34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>642.9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>642.91</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>642.91999999999996</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>642.92999999999995</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>642.94000000000005</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>1298</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>2678</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>2679</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>2798</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>2799</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>2299</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>2300</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>2752</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>2753</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>3290</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>3291</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>1346</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>2336</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1" t="s">
+        <v>2337</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1" t="s">
+        <v>1402</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1" t="s">
+        <v>1683</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1" t="s">
+        <v>1354</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1" t="s">
+        <v>1714</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>856</v>
       </c>
     </row>
@@ -40061,7 +40066,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41665,7 +41670,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42631,7 +42636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAA8D08-73B3-4AE7-B434-E77EA071DF8A}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
revise diabetes and pulmonary data
</commit_message>
<xml_diff>
--- a/documents/datadictionary/perinatal_ICD_codes_rawdata_01_2022.xlsx
+++ b/documents/datadictionary/perinatal_ICD_codes_rawdata_01_2022.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="8" documentId="8_{9024541E-BFC9-4B55-8A8E-040948A85B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F18C80C-67C7-47AF-952D-BB9248A84BEB}"/>
   <bookViews>
-    <workbookView xWindow="33885" yWindow="630" windowWidth="21360" windowHeight="14220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33885" yWindow="630" windowWidth="21360" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="perinatal_ICD_codes_rawdata_01" sheetId="1" r:id="rId1"/>
@@ -38128,8 +38128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3321D195-85F5-451B-BB8A-48DC8CAF4B8E}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39017,7 +39017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E6D65C-6D8A-4E42-AF7B-9ACBFC461D1A}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated ICD code list
</commit_message>
<xml_diff>
--- a/documents/datadictionary/perinatal_ICD_codes_rawdata_01_2022.xlsx
+++ b/documents/datadictionary/perinatal_ICD_codes_rawdata_01_2022.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a87caf6b30614cd/Documents/ehr-preeclampsia-model/documents/datadictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{9024541E-BFC9-4B55-8A8E-040948A85B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F18C80C-67C7-47AF-952D-BB9248A84BEB}"/>
+  <xr:revisionPtr revIDLastSave="306" documentId="13_ncr:40009_{A4005AD1-E51A-4BCE-8F8B-DFD95862EFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{272C8207-8010-4B08-B8AF-57A50A1D0151}"/>
   <bookViews>
-    <workbookView xWindow="33885" yWindow="630" windowWidth="21360" windowHeight="14220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="perinatal_ICD_codes_rawdata_01" sheetId="1" r:id="rId1"/>
-    <sheet name="diabetes" sheetId="7" r:id="rId2"/>
-    <sheet name="hypertension" sheetId="6" r:id="rId3"/>
+    <sheet name="hypertension" sheetId="6" r:id="rId2"/>
+    <sheet name="diabetes" sheetId="7" r:id="rId3"/>
     <sheet name="multiples" sheetId="3" r:id="rId4"/>
     <sheet name="pe" sheetId="5" r:id="rId5"/>
     <sheet name="pulmonary" sheetId="9" r:id="rId6"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7524" uniqueCount="3773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7518" uniqueCount="3767">
   <si>
     <t>perinatal_dx_code</t>
   </si>
@@ -11325,25 +11325,7 @@
     <t>pulmonary</t>
   </si>
   <si>
-    <t>64.32</t>
-  </si>
-  <si>
-    <t>642.33</t>
-  </si>
-  <si>
-    <t>642.9</t>
-  </si>
-  <si>
-    <t>642.91</t>
-  </si>
-  <si>
-    <t>642.92</t>
-  </si>
-  <si>
-    <t>642.93</t>
-  </si>
-  <si>
-    <t>642.94</t>
+    <t>642.2</t>
   </si>
 </sst>
 </file>
@@ -11486,7 +11468,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -11666,12 +11648,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -11833,16 +11809,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -12203,7 +12176,7 @@
   <dimension ref="A1:D2290"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A169" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38125,11 +38098,1081 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E6D65C-6D8A-4E42-AF7B-9ACBFC461D1A}">
+  <dimension ref="A1:F58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="146" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3723</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3724</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3730</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>642</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>642.01</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>642.02</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>642.03</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>642.04</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>642.11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>642.13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>642.14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3766</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>642.21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>642.23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>642.24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>642.29999999999995</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>642.30999999999995</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>642.32000000000005</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>642.33000000000004</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>642.34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>642.9</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>642.91</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>642.91999999999996</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>642.92999999999995</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>642.94000000000005</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>993</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>957</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>1298</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>2678</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>2679</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1" t="s">
+        <v>1342</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>2798</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>2799</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>2299</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1" t="s">
+        <v>2300</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>2752</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>2753</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>3290</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>3291</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>1346</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>2336</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1" t="s">
+        <v>2337</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1" t="s">
+        <v>922</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1" t="s">
+        <v>1402</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1" t="s">
+        <v>1683</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>854</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1" t="s">
+        <v>1354</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1" t="s">
+        <v>1714</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>3762</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>929</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>3761</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>3763</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3321D195-85F5-451B-BB8A-48DC8CAF4B8E}">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38169,8 +39212,8 @@
       <c r="B2" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>3762</v>
+      <c r="C2" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
@@ -38187,8 +39230,8 @@
       <c r="B3" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>3762</v>
+      <c r="C3" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
@@ -38583,8 +39626,8 @@
       <c r="B25" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>3762</v>
+      <c r="C25" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
@@ -38601,8 +39644,8 @@
       <c r="B26" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>3762</v>
+      <c r="C26" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
@@ -38619,8 +39662,8 @@
       <c r="B27" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>3762</v>
+      <c r="C27" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
@@ -38637,8 +39680,8 @@
       <c r="B28" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>3762</v>
+      <c r="C28" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
@@ -38655,8 +39698,8 @@
       <c r="B29" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>3762</v>
+      <c r="C29" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
@@ -38673,8 +39716,8 @@
       <c r="B30" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>3762</v>
+      <c r="C30" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
@@ -38691,8 +39734,8 @@
       <c r="B31" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>3762</v>
+      <c r="C31" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
@@ -38709,8 +39752,8 @@
       <c r="B32" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>3762</v>
+      <c r="C32" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
@@ -38727,8 +39770,8 @@
       <c r="B33" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>3762</v>
+      <c r="C33" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
@@ -38745,8 +39788,8 @@
       <c r="B34" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>3762</v>
+      <c r="C34" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
@@ -38763,8 +39806,8 @@
       <c r="B35" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>3762</v>
+      <c r="C35" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
@@ -38781,8 +39824,8 @@
       <c r="B36" s="1" t="s">
         <v>3764</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>3762</v>
+      <c r="C36" s="1" t="s">
+        <v>3763</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
@@ -39010,1076 +40053,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E6D65C-6D8A-4E42-AF7B-9ACBFC461D1A}">
-  <dimension ref="A1:F58"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="146" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3723</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3724</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3730</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>642</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>642.01</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>642.02</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>567</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>642.03</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>642.04</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>642.11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>642.13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>642.14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>849</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>642.20000000000005</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>642.21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>642.23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>642.24</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>642.29999999999995</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>642.30999999999995</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>3766</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>3767</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>642.34</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>3768</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>3769</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>3770</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>3771</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>3772</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>1236</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1" t="s">
-        <v>1237</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>993</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1" t="s">
-        <v>994</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>933</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1" t="s">
-        <v>934</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>957</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1" t="s">
-        <v>958</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>1120</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1" t="s">
-        <v>1121</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>1297</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1" t="s">
-        <v>1298</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>2678</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1" t="s">
-        <v>2679</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>1341</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1" t="s">
-        <v>1342</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>2798</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1" t="s">
-        <v>2799</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>2299</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1" t="s">
-        <v>2300</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>2752</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1" t="s">
-        <v>2753</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>3290</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1" t="s">
-        <v>3291</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1" t="s">
-        <v>1235</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>1345</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1" t="s">
-        <v>1346</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>1003</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1" t="s">
-        <v>1004</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>919</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1" t="s">
-        <v>920</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>1023</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1" t="s">
-        <v>1024</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>925</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1" t="s">
-        <v>926</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>2336</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1" t="s">
-        <v>2337</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>1439</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1" t="s">
-        <v>1440</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>921</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1" t="s">
-        <v>922</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>1150</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1" t="s">
-        <v>1151</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>1401</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1" t="s">
-        <v>1402</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>947</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>3763</v>
-      </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1" t="s">
-        <v>948</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>1240</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1" t="s">
-        <v>1241</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>1682</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1" t="s">
-        <v>1683</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>883</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1" t="s">
-        <v>884</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>854</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1" t="s">
-        <v>855</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>1353</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1" t="s">
-        <v>1354</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>1713</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1" t="s">
-        <v>1714</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1" t="s">
-        <v>1231</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>1009</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1" t="s">
-        <v>1010</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>1162</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1" t="s">
-        <v>1163</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>1248</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1" t="s">
-        <v>1249</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>929</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>3761</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>3762</v>
-      </c>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1" t="s">
-        <v>930</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>856</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -40088,7 +40061,7 @@
   <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41692,7 +41665,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add O11 ICD10 codes
</commit_message>
<xml_diff>
--- a/documents/datadictionary/perinatal_ICD_codes_rawdata_01_2022.xlsx
+++ b/documents/datadictionary/perinatal_ICD_codes_rawdata_01_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a87caf6b30614cd/Documents/ehr-preeclampsia-model/documents/datadictionary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haile\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="306" documentId="13_ncr:40009_{A4005AD1-E51A-4BCE-8F8B-DFD95862EFEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{272C8207-8010-4B08-B8AF-57A50A1D0151}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641DA09C-A71F-4077-B2B7-38847FA26FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="perinatal_ICD_codes_rawdata_01" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7518" uniqueCount="3767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7554" uniqueCount="3767">
   <si>
     <t>perinatal_dx_code</t>
   </si>
@@ -38101,7 +38101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E6D65C-6D8A-4E42-AF7B-9ACBFC461D1A}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -41662,10 +41662,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3529DB55-292E-4290-A6A1-693D425C89C7}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42615,6 +42615,126 @@
         <v>946</v>
       </c>
       <c r="F47" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>2336</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3748</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3756</v>
+      </c>
+      <c r="D48" t="s">
+        <v>3732</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2337</v>
+      </c>
+      <c r="F48" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3748</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3756</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3735</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1440</v>
+      </c>
+      <c r="F49" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3748</v>
+      </c>
+      <c r="C50" t="s">
+        <v>3756</v>
+      </c>
+      <c r="D50" t="s">
+        <v>3734</v>
+      </c>
+      <c r="E50" t="s">
+        <v>922</v>
+      </c>
+      <c r="F50" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3748</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3756</v>
+      </c>
+      <c r="D51" t="s">
+        <v>3749</v>
+      </c>
+      <c r="E51" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F51" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3748</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3756</v>
+      </c>
+      <c r="D52" t="s">
+        <v>3749</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1402</v>
+      </c>
+      <c r="F52" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3748</v>
+      </c>
+      <c r="C53" t="s">
+        <v>3756</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3733</v>
+      </c>
+      <c r="E53" t="s">
+        <v>948</v>
+      </c>
+      <c r="F53" t="s">
         <v>856</v>
       </c>
     </row>

</xml_diff>